<commit_message>
add lecture 7 inclass
</commit_message>
<xml_diff>
--- a/assignment_starters/assign2_starter/leaky_iandf_inclass.xlsx
+++ b/assignment_starters/assign2_starter/leaky_iandf_inclass.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremyhogeveen/Dropbox/Fall_2023/teaching/PSY450_650/DSPN_Fall2023_workdir/assignment_starters/assign2_starter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremyhogeveen/Dropbox/Fall_2023/teaching/PSY450_650/DSPN_Fall2023_Git/assignment_starters/assign2_starter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B4FF4B-0980-B240-ACB9-77DDEF8785AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD28E272-3B32-444D-8170-28D626A5ABDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38340" yWindow="4060" windowWidth="22820" windowHeight="14500" xr2:uid="{A937FB6C-C437-524F-A003-58A0D75E6AA6}"/>
+    <workbookView xWindow="2800" yWindow="760" windowWidth="30240" windowHeight="16260" xr2:uid="{A937FB6C-C437-524F-A003-58A0D75E6AA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>dt</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>spike_counter</t>
   </si>
 </sst>
 </file>
@@ -223,6 +226,450 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="149"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.355</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.7195</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.0475500000000002</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.3427950000000002</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.6085155000000002</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.8476639500000003</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.0628975550000002</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.2566077995000002</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3.43094701955</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3.5878523175949999</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.7290670858354997</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.8561603772519497</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.9705443395267546</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4.0734899055740792</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.355</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.7195</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.0475500000000002</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.3427950000000002</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.6085155000000002</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2.8476639500000003</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.0628975550000002</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3.2566077995000002</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3.43094701955</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.5878523175949999</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.7290670858354997</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.8561603772519497</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.9705443395267546</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4.0734899055740792</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1.355</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1.7195</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2.0475500000000002</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2.3427950000000002</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2.6085155000000002</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2.8476639500000003</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>3.0628975550000002</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3.2566077995000002</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3.43094701955</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3.5878523175949999</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3.7290670858354997</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3.8561603772519497</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3.9705443395267546</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>4.0734899055740792</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="148">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1483,16 +1930,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>601663</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>220663</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1817,15 +2264,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0807FA3E-3A7F-9147-8A7C-C0F1B446E459}">
-  <dimension ref="A1:H152"/>
+  <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1850,8 +2297,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1874,15 +2324,22 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <f>IF(B2&lt;50,0,IF(B2&gt;100,0,1))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>SUM(G2:G152)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3">
         <f>$A$2+B2</f>
         <v>1</v>
       </c>
+      <c r="E3">
+        <f>IF(H3=0,0,IF(E2&gt;=$D$2,0,E2 + $A$2*(-1*(E2/$C$2) + $F$2 * (H3 / $C$2))))</f>
+        <v>0</v>
+      </c>
       <c r="G3">
         <f>IF(E3&gt;$D$2,1,0)</f>
         <v>0</v>
@@ -1892,13 +2349,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4">
         <f t="shared" ref="B4:B67" si="1">$A$2+B3</f>
         <v>2</v>
       </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E67" si="2">IF(H4=0,0,IF(E3&gt;=$D$2,0,E3 + $A$2*(-1*(E3/$C$2) + $F$2 * (H4 / $C$2))))</f>
+        <v>0</v>
+      </c>
       <c r="G4">
-        <f t="shared" ref="G4:G67" si="2">IF(E4&gt;$D$2,1,0)</f>
+        <f t="shared" ref="G4:G67" si="3">IF(E4&gt;$D$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="H4">
@@ -1906,13 +2367,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H5">
@@ -1920,13 +2385,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H6">
@@ -1934,13 +2403,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H7">
@@ -1948,13 +2421,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H8">
@@ -1962,13 +2439,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H9">
@@ -1976,13 +2457,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H10">
@@ -1990,13 +2475,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H11">
@@ -2004,13 +2493,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H12">
@@ -2018,13 +2511,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H13">
@@ -2032,13 +2529,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H14">
@@ -2046,13 +2547,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H15">
@@ -2060,13 +2565,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H16">
@@ -2079,8 +2588,12 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H17">
@@ -2093,8 +2606,12 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H18">
@@ -2107,8 +2624,12 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H19">
@@ -2121,8 +2642,12 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H20">
@@ -2135,8 +2660,12 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H21">
@@ -2149,8 +2678,12 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H22">
@@ -2163,8 +2696,12 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H23">
@@ -2177,8 +2714,12 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H24">
@@ -2191,8 +2732,12 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H25">
@@ -2205,8 +2750,12 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H26">
@@ -2219,8 +2768,12 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H27">
@@ -2233,8 +2786,12 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H28">
@@ -2247,8 +2804,12 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H29">
@@ -2261,8 +2822,12 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H30">
@@ -2275,8 +2840,12 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H31">
@@ -2289,8 +2858,12 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H32">
@@ -2303,8 +2876,12 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H33">
@@ -2317,8 +2894,12 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H34">
@@ -2331,8 +2912,12 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H35">
@@ -2345,8 +2930,12 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H36">
@@ -2359,8 +2948,12 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H37">
@@ -2373,8 +2966,12 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H38">
@@ -2387,8 +2984,12 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H39">
@@ -2401,8 +3002,12 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H40">
@@ -2415,8 +3020,12 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H41">
@@ -2429,8 +3038,12 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H42">
@@ -2443,8 +3056,12 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H43">
@@ -2457,8 +3074,12 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H44">
@@ -2471,8 +3092,12 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H45">
@@ -2485,8 +3110,12 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H46">
@@ -2499,8 +3128,12 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H47">
@@ -2513,8 +3146,12 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H48">
@@ -2527,8 +3164,12 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H49">
@@ -2541,8 +3182,12 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H50">
@@ -2555,8 +3200,12 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H51">
@@ -2569,8 +3218,12 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
       <c r="G52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H52">
@@ -2583,8 +3236,12 @@
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
       <c r="G53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H53">
@@ -2597,8 +3254,12 @@
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>1.355</v>
+      </c>
       <c r="G54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H54">
@@ -2611,8 +3272,12 @@
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>1.7195</v>
+      </c>
       <c r="G55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H55">
@@ -2625,8 +3290,12 @@
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>2.0475500000000002</v>
+      </c>
       <c r="G56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H56">
@@ -2639,8 +3308,12 @@
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>2.3427950000000002</v>
+      </c>
       <c r="G57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H57">
@@ -2653,8 +3326,12 @@
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>2.6085155000000002</v>
+      </c>
       <c r="G58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H58">
@@ -2667,8 +3344,12 @@
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>2.8476639500000003</v>
+      </c>
       <c r="G59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H59">
@@ -2681,8 +3362,12 @@
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>3.0628975550000002</v>
+      </c>
       <c r="G60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H60">
@@ -2695,8 +3380,12 @@
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>3.2566077995000002</v>
+      </c>
       <c r="G61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H61">
@@ -2709,8 +3398,12 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>3.43094701955</v>
+      </c>
       <c r="G62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H62">
@@ -2723,8 +3416,12 @@
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>3.5878523175949999</v>
+      </c>
       <c r="G63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H63">
@@ -2737,8 +3434,12 @@
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
+      <c r="E64">
+        <f t="shared" si="2"/>
+        <v>3.7290670858354997</v>
+      </c>
       <c r="G64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H64">
@@ -2751,8 +3452,12 @@
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
+      <c r="E65">
+        <f t="shared" si="2"/>
+        <v>3.8561603772519497</v>
+      </c>
       <c r="G65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H65">
@@ -2765,8 +3470,12 @@
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
+      <c r="E66">
+        <f t="shared" si="2"/>
+        <v>3.9705443395267546</v>
+      </c>
       <c r="G66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H66">
@@ -2779,1202 +3488,1546 @@
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
+      <c r="E67">
+        <f t="shared" si="2"/>
+        <v>4.0734899055740792</v>
+      </c>
       <c r="G67">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67:H130" si="3">IF(B67&lt;50,0,IF(B67&gt;100,0,1))</f>
+        <f t="shared" ref="H67:H130" si="4">IF(B67&lt;50,0,IF(B67&gt;100,0,1))</f>
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68">
-        <f t="shared" ref="B68:B131" si="4">$A$2+B67</f>
+        <f t="shared" ref="B68:B131" si="5">$A$2+B67</f>
         <v>66</v>
       </c>
+      <c r="E68">
+        <f t="shared" ref="E68:E131" si="6">IF(H68=0,0,IF(E67&gt;=$D$2,0,E67 + $A$2*(-1*(E67/$C$2) + $F$2 * (H68 / $C$2))))</f>
+        <v>0</v>
+      </c>
       <c r="G68">
-        <f t="shared" ref="G68:G131" si="5">IF(E68&gt;$D$2,1,0)</f>
+        <f t="shared" ref="G68:G131" si="7">IF(E68&gt;$D$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="H68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>67</v>
       </c>
+      <c r="E69">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
       <c r="G69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>68</v>
       </c>
+      <c r="E70">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
       <c r="G70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>69</v>
       </c>
+      <c r="E71">
+        <f t="shared" si="6"/>
+        <v>1.355</v>
+      </c>
       <c r="G71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>70</v>
       </c>
+      <c r="E72">
+        <f t="shared" si="6"/>
+        <v>1.7195</v>
+      </c>
       <c r="G72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>71</v>
       </c>
+      <c r="E73">
+        <f t="shared" si="6"/>
+        <v>2.0475500000000002</v>
+      </c>
       <c r="G73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72</v>
       </c>
+      <c r="E74">
+        <f t="shared" si="6"/>
+        <v>2.3427950000000002</v>
+      </c>
       <c r="G74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>73</v>
       </c>
+      <c r="E75">
+        <f t="shared" si="6"/>
+        <v>2.6085155000000002</v>
+      </c>
       <c r="G75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74</v>
       </c>
+      <c r="E76">
+        <f t="shared" si="6"/>
+        <v>2.8476639500000003</v>
+      </c>
       <c r="G76">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
+      <c r="E77">
+        <f t="shared" si="6"/>
+        <v>3.0628975550000002</v>
+      </c>
       <c r="G77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>76</v>
       </c>
+      <c r="E78">
+        <f t="shared" si="6"/>
+        <v>3.2566077995000002</v>
+      </c>
       <c r="G78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>77</v>
       </c>
+      <c r="E79">
+        <f t="shared" si="6"/>
+        <v>3.43094701955</v>
+      </c>
       <c r="G79">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>78</v>
       </c>
+      <c r="E80">
+        <f t="shared" si="6"/>
+        <v>3.5878523175949999</v>
+      </c>
       <c r="G80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>79</v>
       </c>
+      <c r="E81">
+        <f t="shared" si="6"/>
+        <v>3.7290670858354997</v>
+      </c>
       <c r="G81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>80</v>
       </c>
+      <c r="E82">
+        <f t="shared" si="6"/>
+        <v>3.8561603772519497</v>
+      </c>
       <c r="G82">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
+      <c r="E83">
+        <f t="shared" si="6"/>
+        <v>3.9705443395267546</v>
+      </c>
       <c r="G83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>82</v>
       </c>
+      <c r="E84">
+        <f t="shared" si="6"/>
+        <v>4.0734899055740792</v>
+      </c>
       <c r="G84">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="H84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>83</v>
       </c>
+      <c r="E85">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G85">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>84</v>
       </c>
+      <c r="E86">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
       <c r="G86">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>85</v>
       </c>
+      <c r="E87">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
       <c r="G87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>86</v>
       </c>
+      <c r="E88">
+        <f t="shared" si="6"/>
+        <v>1.355</v>
+      </c>
       <c r="G88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>87</v>
       </c>
+      <c r="E89">
+        <f t="shared" si="6"/>
+        <v>1.7195</v>
+      </c>
       <c r="G89">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>88</v>
       </c>
+      <c r="E90">
+        <f t="shared" si="6"/>
+        <v>2.0475500000000002</v>
+      </c>
       <c r="G90">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>89</v>
       </c>
+      <c r="E91">
+        <f t="shared" si="6"/>
+        <v>2.3427950000000002</v>
+      </c>
       <c r="G91">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>90</v>
       </c>
+      <c r="E92">
+        <f t="shared" si="6"/>
+        <v>2.6085155000000002</v>
+      </c>
       <c r="G92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>91</v>
       </c>
+      <c r="E93">
+        <f t="shared" si="6"/>
+        <v>2.8476639500000003</v>
+      </c>
       <c r="G93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>92</v>
       </c>
+      <c r="E94">
+        <f t="shared" si="6"/>
+        <v>3.0628975550000002</v>
+      </c>
       <c r="G94">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>93</v>
       </c>
+      <c r="E95">
+        <f t="shared" si="6"/>
+        <v>3.2566077995000002</v>
+      </c>
       <c r="G95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>94</v>
       </c>
+      <c r="E96">
+        <f t="shared" si="6"/>
+        <v>3.43094701955</v>
+      </c>
       <c r="G96">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>95</v>
       </c>
+      <c r="E97">
+        <f t="shared" si="6"/>
+        <v>3.5878523175949999</v>
+      </c>
       <c r="G97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H97">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B98">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>96</v>
       </c>
+      <c r="E98">
+        <f t="shared" si="6"/>
+        <v>3.7290670858354997</v>
+      </c>
       <c r="G98">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B99">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>97</v>
       </c>
+      <c r="E99">
+        <f t="shared" si="6"/>
+        <v>3.8561603772519497</v>
+      </c>
       <c r="G99">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H99">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>98</v>
       </c>
+      <c r="E100">
+        <f t="shared" si="6"/>
+        <v>3.9705443395267546</v>
+      </c>
       <c r="G100">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H100">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>99</v>
       </c>
+      <c r="E101">
+        <f t="shared" si="6"/>
+        <v>4.0734899055740792</v>
+      </c>
       <c r="G101">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="H101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B102">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
+      <c r="E102">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G102">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B103">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>101</v>
       </c>
+      <c r="E103">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G103">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H103">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B104">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>102</v>
       </c>
+      <c r="E104">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G104">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H104">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B105">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>103</v>
       </c>
+      <c r="E105">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G105">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H105">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B106">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
+      <c r="E106">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G106">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H106">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>105</v>
       </c>
+      <c r="E107">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H107">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>106</v>
       </c>
+      <c r="E108">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G108">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H108">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="109" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B109">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>107</v>
       </c>
+      <c r="E109">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G109">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H109">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B110">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>108</v>
       </c>
+      <c r="E110">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G110">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H110">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>109</v>
       </c>
+      <c r="E111">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G111">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H111">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="112" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B112">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>110</v>
       </c>
+      <c r="E112">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G112">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H112">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B113">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>111</v>
       </c>
+      <c r="E113">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G113">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H113">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="114" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B114">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>112</v>
       </c>
+      <c r="E114">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G114">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H114">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="115" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B115">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>113</v>
       </c>
+      <c r="E115">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G115">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H115">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B116">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>114</v>
       </c>
+      <c r="E116">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G116">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H116">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B117">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>115</v>
       </c>
+      <c r="E117">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G117">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H117">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B118">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>116</v>
       </c>
+      <c r="E118">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G118">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H118">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="119" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B119">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>117</v>
       </c>
+      <c r="E119">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G119">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H119">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B120">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>118</v>
       </c>
+      <c r="E120">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G120">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H120">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B121">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119</v>
       </c>
+      <c r="E121">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G121">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="122" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B122">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>120</v>
       </c>
+      <c r="E122">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G122">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H122">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="123" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>121</v>
       </c>
+      <c r="E123">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B124">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>122</v>
       </c>
+      <c r="E124">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G124">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H124">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B125">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>123</v>
       </c>
+      <c r="E125">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G125">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H125">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B126">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>124</v>
       </c>
+      <c r="E126">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G126">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H126">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B127">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>125</v>
       </c>
+      <c r="E127">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G127">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>126</v>
       </c>
+      <c r="E128">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G128">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B129">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>127</v>
       </c>
+      <c r="E129">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G129">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H129">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B130">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>128</v>
       </c>
+      <c r="E130">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G130">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H130">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="131" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B131">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>129</v>
       </c>
+      <c r="E131">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="G131">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H131">
-        <f t="shared" ref="H131:H152" si="6">IF(B131&lt;50,0,IF(B131&gt;100,0,1))</f>
+        <f t="shared" ref="H131:H152" si="8">IF(B131&lt;50,0,IF(B131&gt;100,0,1))</f>
         <v>0</v>
       </c>
     </row>
     <row r="132" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B132">
-        <f t="shared" ref="B132:B150" si="7">$A$2+B131</f>
+        <f t="shared" ref="B132:B150" si="9">$A$2+B131</f>
         <v>130</v>
       </c>
+      <c r="E132">
+        <f t="shared" ref="E132:E152" si="10">IF(H132=0,0,IF(E131&gt;=$D$2,0,E131 + $A$2*(-1*(E131/$C$2) + $F$2 * (H132 / $C$2))))</f>
+        <v>0</v>
+      </c>
       <c r="G132">
-        <f t="shared" ref="G132:G150" si="8">IF(E132&gt;$D$2,1,0)</f>
+        <f t="shared" ref="G132:G150" si="11">IF(E132&gt;$D$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="H132">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="133" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B133">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>131</v>
       </c>
+      <c r="E133">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G133">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H133">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H133">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="134" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B134">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>132</v>
       </c>
+      <c r="E134">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G134">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H134">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H134">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="135" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B135">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>133</v>
       </c>
+      <c r="E135">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G135">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H135">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H135">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="136" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B136">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>134</v>
       </c>
+      <c r="E136">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G136">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H136">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H136">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="137" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B137">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>135</v>
       </c>
+      <c r="E137">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G137">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H137">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H137">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B138">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>136</v>
       </c>
+      <c r="E138">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G138">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H138">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H138">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="139" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B139">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>137</v>
       </c>
+      <c r="E139">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G139">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H139">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H139">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="140" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B140">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>138</v>
       </c>
+      <c r="E140">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G140">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H140">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H140">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="141" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B141">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>139</v>
       </c>
+      <c r="E141">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G141">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H141">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H141">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="142" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B142">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>140</v>
       </c>
+      <c r="E142">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G142">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H142">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H142">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="143" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B143">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>141</v>
       </c>
+      <c r="E143">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G143">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H143">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H143">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="144" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B144">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>142</v>
       </c>
+      <c r="E144">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G144">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H144">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H144">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="145" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B145">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>143</v>
       </c>
+      <c r="E145">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G145">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H145">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H145">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="146" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B146">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>144</v>
       </c>
+      <c r="E146">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G146">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H146">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H146">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="147" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B147">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>145</v>
       </c>
+      <c r="E147">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G147">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H147">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H147">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="148" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B148">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>146</v>
       </c>
+      <c r="E148">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G148">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H148">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H148">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="149" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B149">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>147</v>
       </c>
+      <c r="E149">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G149">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H149">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H149">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="150" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B150">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>148</v>
       </c>
+      <c r="E150">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G150">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H150">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H150">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="151" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B151">
-        <f t="shared" ref="B151:B152" si="9">$A$2+B150</f>
+        <f t="shared" ref="B151:B152" si="12">$A$2+B150</f>
         <v>149</v>
       </c>
+      <c r="E151">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G151">
-        <f t="shared" ref="G151:G152" si="10">IF(E151&gt;$D$2,1,0)</f>
+        <f t="shared" ref="G151:G152" si="13">IF(E151&gt;$D$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="H151">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="152" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B152">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>150</v>
       </c>
+      <c r="E152">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="G152">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H152">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>